<commit_message>
mail listesi gizlendi ve ihale adımlarındaki yazdır buttonları silindi
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/SentFile/saskom ltd şti-24.03.2018-Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/SentFile/saskom ltd şti-24.03.2018-Malzeme_Fiyat_Listesi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>SIRA</t>
   </si>
@@ -72,34 +72,16 @@
     <t>saskom ltd şti</t>
   </si>
   <si>
-    <t>El ile sert toprak kazılması (kil, siltli, kumlu ve gevşek kil, killi kum ve çakıl, kürekle atılabilen taşlı toprak ve benzeri zeminler)</t>
-  </si>
-  <si>
-    <t>m³</t>
-  </si>
-  <si>
-    <t>Dolgu altının sürülmesi</t>
-  </si>
-  <si>
-    <t>Bnm²</t>
-  </si>
-  <si>
-    <t>Kazı ve dolgu alanında makine ile temizleme ve sökme işi yapılması</t>
-  </si>
-  <si>
-    <t>Yzm²</t>
-  </si>
-  <si>
-    <t>Ağ Görüntü Kayıt Cihazı (NVR)</t>
+    <t>Ağ görüntü cihazı NVR 48</t>
   </si>
   <si>
     <t>adet</t>
   </si>
   <si>
-    <t>Dış Ortam Sabit Box/Bullet Tipi Kamera (Kamera Muhafazası ve Infrared LED Projektör dahil)</t>
+    <t>Dış ortam sabit box/bullet tipi led</t>
   </si>
   <si>
-    <t>Saha Anahtarı (TİP1)</t>
+    <t>hareketli kamera</t>
   </si>
 </sst>
 </file>
@@ -1043,13 +1025,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E7" s="9">
         <v>1</v>
@@ -1061,20 +1043,20 @@
         <v>18</v>
       </c>
       <c r="H7" s="10">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E8" s="13">
         <v>2</v>
@@ -1083,111 +1065,60 @@
         <v>19</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8" s="14">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="14">
-        <v>345</v>
+        <v>60</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>44</v>
-      </c>
-      <c r="E10" s="13">
-        <v>4</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="14">
-        <v>546</v>
-      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>45</v>
-      </c>
-      <c r="E11" s="13">
-        <v>5</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="14">
-        <v>56</v>
-      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="15"/>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>46</v>
-      </c>
-      <c r="E12" s="13">
-        <v>6</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="14">
-        <v>76</v>
-      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="15"/>
       <c r="J12" s="16"/>
     </row>

</xml_diff>